<commit_message>
- everything should be ready for user - improve and make shine html - fix bugs
</commit_message>
<xml_diff>
--- a/Ads – AngularJS Practical Project/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads – AngularJS Practical Project/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,9 +760,7 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6">
-        <v>15</v>
-      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="12" t="s">
         <v>56</v>
       </c>
@@ -772,9 +770,7 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
-        <v>44</v>
-      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
@@ -792,9 +788,7 @@
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5">
-        <v>10</v>
-      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
@@ -804,9 +798,7 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
@@ -816,9 +808,7 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5">
-        <v>5</v>
-      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
@@ -828,9 +818,7 @@
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5">
-        <v>5</v>
-      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
@@ -840,9 +828,7 @@
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5">
-        <v>5</v>
-      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
@@ -852,9 +838,7 @@
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
-        <v>5</v>
-      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
@@ -864,9 +848,7 @@
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="5">
-        <v>5</v>
-      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
@@ -876,9 +858,7 @@
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5">
-        <v>5</v>
-      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
@@ -1008,9 +988,7 @@
       <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="5">
-        <v>5</v>
-      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
@@ -1020,9 +998,7 @@
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5">
-        <v>5</v>
-      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1188,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
- JS-SPA-Self-Evaluation-Protocol-update - my last commit for this project
</commit_message>
<xml_diff>
--- a/Ads – AngularJS Practical Project/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads – AngularJS Practical Project/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>https://github.com/dimitarIT/AngularJS/tree/master/Ads%20%E2%80%93%20AngularJS%20Practical%20Project</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +763,9 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>15</v>
+      </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
       </c>
@@ -770,7 +775,9 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>65</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
@@ -788,221 +795,309 @@
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>10</v>
+      </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
@@ -1188,7 +1283,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>